<commit_message>
- finish documentation (except for screenshots and deprecation warnings)  - replace sample files
</commit_message>
<xml_diff>
--- a/docs/assets/data_model_templates/rosetta (rosetta)/properties.xlsx
+++ b/docs/assets/data_model_templates/rosetta (rosetta)/properties.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/docs/assets/data_model_templates/rosetta (rosetta)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16B0125-440F-3342-85DE-269EC4BA61FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428EA52B-3D64-674C-8A37-65A164E7564B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="760" windowWidth="29580" windowHeight="17820" xr2:uid="{352B9572-BD89-B646-9758-957DE76BD52A}"/>
+    <workbookView xWindow="0" yWindow="3180" windowWidth="34560" windowHeight="17820" xr2:uid="{352B9572-BD89-B646-9758-957DE76BD52A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,33 +32,455 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Johannes Nussbaum</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CCE0D910-B5B4-984B-B270-F2E970013FFE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Unique identifier for the property</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{EAC90691-C48C-1248-8FED-F509390B19E3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>one language mandatory</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Label of the property that will be displayed in DSP-APP. Should be rather short. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{1E3F62D4-01AE-4549-B0CE-527D4AB892A8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">optional
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Description of the property. Can be longer than the label.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{3762951F-32E6-5540-A28D-060817FA28E1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">The base property/ies that this property is derived from. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Must be one of the values listed in the documentation.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">If more than one: separated by commas. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">(This is the "super" in the JSON file.) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{009871A6-31A5-C74B-834F-CF498F3E2165}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Target value of this property. Must be one of the values listed in the documentation. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">If the property is derived from hasValue, the type of the property must be further specified by the object it takes, e.g. TextValue, ListValue, or IntValue. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>If the property is derived from hasLinkTo, the object specifies the resource class that this property refers to.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{23406945-B931-FE47-8D2A-D6C0E1212B1F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">The graphic component, defines how this property should be displayed. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Depends on the value of "object".</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Read the documentation of the respective "object" to learn which "gui_element" can be used.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{0D262A12-08A3-6D4F-BFAC-8F678E499BC1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">only mandatory for lists
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Some "gui_elements" need further specification. Read the documentation of the respective "object" to learn if your "gui_element" needs a "gui_attributes".
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Form: "attr: value, attr: value". </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="151">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>super</t>
-  </si>
-  <si>
     <t>object</t>
   </si>
   <si>
-    <t>en</t>
-  </si>
-  <si>
-    <t>de</t>
-  </si>
-  <si>
-    <t>fr</t>
-  </si>
-  <si>
-    <t>it</t>
-  </si>
-  <si>
-    <t>rm</t>
-  </si>
-  <si>
     <t>comment_en</t>
   </si>
   <si>
@@ -486,13 +908,31 @@
   </si>
   <si>
     <t>max: 25.0, min: 0</t>
+  </si>
+  <si>
+    <t>label_en</t>
+  </si>
+  <si>
+    <t>label_de</t>
+  </si>
+  <si>
+    <t>label_fr</t>
+  </si>
+  <si>
+    <t>label_it</t>
+  </si>
+  <si>
+    <t>label_rm</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -504,6 +944,36 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -526,14 +996,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -845,764 +1318,774 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB295ED-2B92-7F4D-AD0D-5345A9E34A8B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB295ED-2B92-7F4D-AD0D-5345A9E34A8B}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:N1048576"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" customWidth="1"/>
-    <col min="7" max="7" width="5.5" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" customWidth="1"/>
-    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.83203125" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="O2" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="O3" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" t="s">
         <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" t="s">
-        <v>36</v>
-      </c>
-      <c r="O4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" t="s">
+        <v>33</v>
       </c>
       <c r="N5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
+        <v>41</v>
+      </c>
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" t="s">
+        <v>19</v>
       </c>
       <c r="N6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="L7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" t="s">
+        <v>19</v>
       </c>
       <c r="N7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="O7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" t="s">
-        <v>57</v>
+        <v>51</v>
+      </c>
+      <c r="L8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" t="s">
+        <v>11</v>
       </c>
       <c r="N8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="O8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" t="s">
-        <v>62</v>
+        <v>56</v>
+      </c>
+      <c r="L9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" t="s">
+        <v>53</v>
       </c>
       <c r="N9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="L10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" t="s">
+        <v>19</v>
       </c>
       <c r="N10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" t="s">
-        <v>71</v>
+        <v>65</v>
+      </c>
+      <c r="L11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" t="s">
+        <v>62</v>
       </c>
       <c r="N11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" t="s">
-        <v>76</v>
+        <v>70</v>
+      </c>
+      <c r="L12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" t="s">
+        <v>67</v>
       </c>
       <c r="N12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="L13" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" t="s">
+        <v>26</v>
       </c>
       <c r="N13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="O13" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" t="s">
+        <v>78</v>
+      </c>
+      <c r="L14" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" t="s">
+        <v>77</v>
+      </c>
+      <c r="N14" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" t="s">
         <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" t="s">
-        <v>84</v>
-      </c>
-      <c r="N14" t="s">
-        <v>21</v>
-      </c>
-      <c r="O14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" t="s">
-        <v>89</v>
+        <v>83</v>
+      </c>
+      <c r="L15" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" t="s">
+        <v>19</v>
       </c>
       <c r="N15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="O15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
-      </c>
-      <c r="E16" t="s">
-        <v>93</v>
-      </c>
-      <c r="F16" t="s">
-        <v>94</v>
+        <v>88</v>
+      </c>
+      <c r="L16" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" t="s">
+        <v>67</v>
       </c>
       <c r="N16" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+      <c r="L17" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" t="s">
+        <v>23</v>
+      </c>
+      <c r="O17" t="s">
         <v>24</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" t="s">
-        <v>96</v>
-      </c>
-      <c r="F17" t="s">
-        <v>97</v>
-      </c>
-      <c r="N17" t="s">
-        <v>29</v>
-      </c>
-      <c r="O17" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" t="s">
-        <v>99</v>
-      </c>
-      <c r="F18" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+      <c r="L18" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" t="s">
+        <v>19</v>
       </c>
       <c r="N18" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" t="s">
+        <v>99</v>
+      </c>
+      <c r="L19" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" t="s">
+        <v>96</v>
+      </c>
+      <c r="N19" t="s">
+        <v>15</v>
+      </c>
+      <c r="O19" t="s">
         <v>16</v>
-      </c>
-      <c r="C19" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" t="s">
-        <v>103</v>
-      </c>
-      <c r="E19" t="s">
-        <v>104</v>
-      </c>
-      <c r="F19" t="s">
-        <v>105</v>
-      </c>
-      <c r="N19" t="s">
-        <v>21</v>
-      </c>
-      <c r="O19" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" t="s">
-        <v>109</v>
-      </c>
-      <c r="F20" t="s">
-        <v>110</v>
+        <v>104</v>
+      </c>
+      <c r="L20" t="s">
+        <v>18</v>
+      </c>
+      <c r="M20" t="s">
+        <v>101</v>
       </c>
       <c r="N20" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
       <c r="D21" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" t="s">
-        <v>114</v>
-      </c>
-      <c r="F21" t="s">
-        <v>115</v>
+        <v>109</v>
+      </c>
+      <c r="L21" t="s">
+        <v>18</v>
+      </c>
+      <c r="M21" t="s">
+        <v>19</v>
       </c>
       <c r="N21" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>111</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
       <c r="D22" t="s">
-        <v>117</v>
-      </c>
-      <c r="E22" t="s">
-        <v>118</v>
-      </c>
-      <c r="F22" t="s">
-        <v>117</v>
+        <v>111</v>
+      </c>
+      <c r="L22" t="s">
+        <v>18</v>
+      </c>
+      <c r="M22" t="s">
+        <v>19</v>
       </c>
       <c r="N22" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>114</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" t="s">
-        <v>121</v>
-      </c>
-      <c r="F23" t="s">
-        <v>122</v>
+        <v>116</v>
+      </c>
+      <c r="L23" t="s">
+        <v>18</v>
+      </c>
+      <c r="M23" t="s">
+        <v>19</v>
       </c>
       <c r="N23" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>118</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>118</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
-      </c>
-      <c r="E24" t="s">
-        <v>124</v>
-      </c>
-      <c r="F24" t="s">
-        <v>125</v>
+        <v>119</v>
+      </c>
+      <c r="L24" t="s">
+        <v>18</v>
+      </c>
+      <c r="M24" t="s">
+        <v>19</v>
       </c>
       <c r="N24" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>122</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E25" t="s">
-        <v>129</v>
-      </c>
-      <c r="F25" t="s">
-        <v>130</v>
+        <v>124</v>
+      </c>
+      <c r="L25" t="s">
+        <v>18</v>
+      </c>
+      <c r="M25" t="s">
+        <v>121</v>
       </c>
       <c r="N25" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="O25" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" t="s">
+        <v>130</v>
+      </c>
+      <c r="L26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M26" t="s">
+        <v>127</v>
+      </c>
+      <c r="N26" t="s">
+        <v>15</v>
+      </c>
+      <c r="O26" t="s">
         <v>16</v>
-      </c>
-      <c r="C26" t="s">
-        <v>133</v>
-      </c>
-      <c r="D26" t="s">
-        <v>134</v>
-      </c>
-      <c r="E26" t="s">
-        <v>135</v>
-      </c>
-      <c r="F26" t="s">
-        <v>136</v>
-      </c>
-      <c r="N26" t="s">
-        <v>21</v>
-      </c>
-      <c r="O26" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>133</v>
       </c>
       <c r="C27" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D27" t="s">
-        <v>139</v>
-      </c>
-      <c r="E27" t="s">
-        <v>140</v>
-      </c>
-      <c r="F27" t="s">
-        <v>139</v>
+        <v>133</v>
+      </c>
+      <c r="L27" t="s">
+        <v>18</v>
+      </c>
+      <c r="M27" t="s">
+        <v>132</v>
       </c>
       <c r="N27" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" t="s">
+        <v>137</v>
+      </c>
+      <c r="L28" t="s">
+        <v>18</v>
+      </c>
+      <c r="M28" t="s">
+        <v>62</v>
+      </c>
+      <c r="N28" t="s">
+        <v>23</v>
+      </c>
+      <c r="O28" t="s">
         <v>24</v>
-      </c>
-      <c r="C28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" t="s">
-        <v>143</v>
-      </c>
-      <c r="E28" t="s">
-        <v>143</v>
-      </c>
-      <c r="F28" t="s">
-        <v>143</v>
-      </c>
-      <c r="N28" t="s">
-        <v>29</v>
-      </c>
-      <c r="O28" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" t="s">
+        <v>142</v>
+      </c>
+      <c r="L29" t="s">
+        <v>18</v>
+      </c>
+      <c r="M29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N29" t="s">
+        <v>143</v>
+      </c>
+      <c r="O29" t="s">
         <v>144</v>
       </c>
-      <c r="B29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" t="s">
-        <v>145</v>
-      </c>
-      <c r="D29" t="s">
-        <v>146</v>
-      </c>
-      <c r="E29" t="s">
-        <v>147</v>
-      </c>
-      <c r="F29" t="s">
-        <v>148</v>
-      </c>
-      <c r="N29" t="s">
-        <v>149</v>
-      </c>
-      <c r="O29" t="s">
-        <v>150</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L1" r:id="rId1" location="super" xr:uid="{C4AC85ED-2737-0644-B535-7723C73DAA7A}"/>
+    <hyperlink ref="N1" r:id="rId2" location="object-gui_element-gui_attributes" xr:uid="{7AB55988-1066-3349-92C2-F503DA7A0F75}"/>
+    <hyperlink ref="M1" r:id="rId3" location="object-gui_element-gui_attributes" xr:uid="{CE33BFD0-D434-134A-A777-EE94E7AC4C74}"/>
+    <hyperlink ref="O1" r:id="rId4" location="object-gui_element-gui_attributes" xr:uid="{C50E7BE7-3EAF-FC45-B133-174C96D20DFF}"/>
+    <hyperlink ref="G1" r:id="rId5" location="comments" xr:uid="{F0DAEBC5-CA77-0B49-B098-42C0474DB112}"/>
+    <hyperlink ref="B1" r:id="rId6" location="labels" xr:uid="{6B82D597-CFF8-E742-9EFA-6B638D35BAFD}"/>
+    <hyperlink ref="A1" r:id="rId7" location="name_1" xr:uid="{511D6563-BCE4-9F4E-8B18-5F9B208025D6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adapt test data and screenshots
</commit_message>
<xml_diff>
--- a/docs/assets/data_model_templates/rosetta (rosetta)/properties.xlsx
+++ b/docs/assets/data_model_templates/rosetta (rosetta)/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/dsp-tools/docs/assets/data_model_templates/rosetta (rosetta)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D486172C-7999-6645-BB1D-EBFA2158D7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374A97F3-5ED9-6C42-811E-7850CA1454A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="3600" windowWidth="27640" windowHeight="16940" xr2:uid="{39EADD64-DA63-9448-899F-8078B27ECEBC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{39EADD64-DA63-9448-899F-8078B27ECEBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -374,7 +366,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="149">
   <si>
     <t>label_de</t>
   </si>
@@ -442,9 +434,6 @@
     <t>hasValue</t>
   </si>
   <si>
-    <t>TextValue</t>
-  </si>
-  <si>
     <t>SimpleText</t>
   </si>
   <si>
@@ -487,18 +476,12 @@
     <t>Commentaire</t>
   </si>
   <si>
-    <t>Richtext</t>
-  </si>
-  <si>
     <t>Copyright</t>
   </si>
   <si>
     <t>Droits d’auteur</t>
   </si>
   <si>
-    <t xml:space="preserve">maxlength: 128, size: 64 </t>
-  </si>
-  <si>
     <t>Künstler:in</t>
   </si>
   <si>
@@ -571,9 +554,6 @@
     <t>Numéro d’inventaire</t>
   </si>
   <si>
-    <t>maxlength: 80, size: 25</t>
-  </si>
-  <si>
     <t>Ort</t>
   </si>
   <si>
@@ -827,13 +807,19 @@
   </si>
   <si>
     <t>Number of children</t>
+  </si>
+  <si>
+    <t>UnformattedTextValue</t>
+  </si>
+  <si>
+    <t>FormattedTextValue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -872,6 +858,13 @@
       <name val="+mn-lt"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -894,10 +887,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1216,7 +1210,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1225,23 +1219,24 @@
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.5" customWidth="1"/>
     <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" customWidth="1"/>
     <col min="12" max="12" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1285,10 +1280,10 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1311,10 +1306,10 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -1326,128 +1321,113 @@
         <v>21</v>
       </c>
       <c r="M3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" t="s">
         <v>26</v>
       </c>
-      <c r="L4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>27</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>28</v>
-      </c>
-      <c r="O4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>33</v>
-      </c>
-      <c r="N5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
       <c r="L6" t="s">
         <v>21</v>
       </c>
       <c r="M6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" t="s">
-        <v>37</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L7" t="s">
         <v>21</v>
       </c>
-      <c r="M7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O7" t="s">
-        <v>40</v>
+      <c r="M7" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M8" t="s">
         <v>16</v>
@@ -1461,140 +1441,137 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" t="s">
+        <v>43</v>
+      </c>
+      <c r="N9" t="s">
         <v>44</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" t="s">
-        <v>46</v>
-      </c>
-      <c r="N9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L10" t="s">
         <v>21</v>
       </c>
       <c r="M10" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" t="s">
-        <v>37</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L11" t="s">
         <v>21</v>
       </c>
       <c r="M11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="N11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" t="s">
         <v>53</v>
-      </c>
-      <c r="D12" t="s">
-        <v>54</v>
-      </c>
-      <c r="L12" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" t="s">
-        <v>55</v>
-      </c>
-      <c r="N12" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L13" t="s">
         <v>21</v>
       </c>
       <c r="M13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="O13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L14" t="s">
         <v>15</v>
       </c>
       <c r="M14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N14" t="s">
         <v>17</v>
@@ -1605,120 +1582,105 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L15" t="s">
         <v>21</v>
       </c>
-      <c r="M15" t="s">
-        <v>22</v>
-      </c>
-      <c r="N15" t="s">
-        <v>23</v>
-      </c>
-      <c r="O15" t="s">
-        <v>65</v>
+      <c r="M15" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L16" t="s">
         <v>21</v>
       </c>
       <c r="M16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="L17" t="s">
         <v>21</v>
       </c>
-      <c r="M17" t="s">
-        <v>22</v>
-      </c>
-      <c r="N17" t="s">
-        <v>23</v>
-      </c>
-      <c r="O17" t="s">
-        <v>24</v>
+      <c r="M17" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="L18" t="s">
         <v>21</v>
       </c>
-      <c r="M18" t="s">
-        <v>22</v>
-      </c>
-      <c r="N18" t="s">
-        <v>37</v>
+      <c r="M18" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="L19" t="s">
         <v>15</v>
       </c>
       <c r="M19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="N19" t="s">
         <v>17</v>
@@ -1729,163 +1691,151 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="L20" t="s">
         <v>21</v>
       </c>
       <c r="M20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="N20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B21" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L21" t="s">
         <v>21</v>
       </c>
-      <c r="M21" t="s">
-        <v>22</v>
-      </c>
-      <c r="N21" t="s">
-        <v>37</v>
+      <c r="M21" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L22" t="s">
         <v>21</v>
       </c>
-      <c r="M22" t="s">
-        <v>22</v>
-      </c>
-      <c r="N22" t="s">
-        <v>37</v>
+      <c r="M22" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B23" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L23" t="s">
         <v>21</v>
       </c>
-      <c r="M23" t="s">
-        <v>22</v>
-      </c>
-      <c r="N23" t="s">
-        <v>37</v>
+      <c r="M23" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="L24" t="s">
         <v>21</v>
       </c>
-      <c r="M24" t="s">
-        <v>22</v>
-      </c>
-      <c r="N24" t="s">
-        <v>37</v>
+      <c r="M24" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D25" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L25" t="s">
         <v>21</v>
       </c>
       <c r="M25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="N25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="L26" t="s">
         <v>15</v>
       </c>
       <c r="M26" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="N26" t="s">
         <v>17</v>
@@ -1896,77 +1846,77 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="L27" t="s">
         <v>21</v>
       </c>
       <c r="M27" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="N27" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="L28" t="s">
         <v>21</v>
       </c>
       <c r="M28" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="N28" t="s">
+        <v>22</v>
+      </c>
+      <c r="O28" t="s">
         <v>23</v>
-      </c>
-      <c r="O28" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B29" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" t="s">
+        <v>96</v>
+      </c>
+      <c r="L29" t="s">
+        <v>21</v>
+      </c>
+      <c r="M29" t="s">
+        <v>97</v>
+      </c>
+      <c r="N29" t="s">
+        <v>98</v>
+      </c>
+      <c r="O29" t="s">
         <v>99</v>
-      </c>
-      <c r="D29" t="s">
-        <v>100</v>
-      </c>
-      <c r="L29" t="s">
-        <v>21</v>
-      </c>
-      <c r="M29" t="s">
-        <v>101</v>
-      </c>
-      <c r="N29" t="s">
-        <v>102</v>
-      </c>
-      <c r="O29" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(excel2json): add optional column "subject" to properties.xlsx (DEV-3253) (#777)
</commit_message>
<xml_diff>
--- a/docs/assets/data_model_templates/rosetta (rosetta)/properties.xlsx
+++ b/docs/assets/data_model_templates/rosetta (rosetta)/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/docs/assets/data_model_templates/rosetta (rosetta)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D486172C-7999-6645-BB1D-EBFA2158D7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADD7F20-3DF7-0F4F-A598-8DFEF1279E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="3600" windowWidth="27640" windowHeight="16940" xr2:uid="{39EADD64-DA63-9448-899F-8078B27ECEBC}"/>
+    <workbookView xWindow="22520" yWindow="5660" windowWidth="27640" windowHeight="16940" xr2:uid="{39EADD64-DA63-9448-899F-8078B27ECEBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -263,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{D3FBF9CF-C152-F14C-BAC2-96F9D75C9E8D}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{D3FBF9CF-C152-F14C-BAC2-96F9D75C9E8D}">
       <text>
         <r>
           <rPr>
@@ -316,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{3FCB58FD-3EA0-D649-A225-B6DF2A08C021}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{3FCB58FD-3EA0-D649-A225-B6DF2A08C021}">
       <text>
         <r>
           <rPr>
@@ -374,7 +373,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="152">
   <si>
     <t>label_de</t>
   </si>
@@ -827,6 +826,9 @@
   </si>
   <si>
     <t>Number of children</t>
+  </si>
+  <si>
+    <t>subject</t>
   </si>
 </sst>
 </file>
@@ -1213,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C6BB55-8531-3D43-8AA9-4A28D8869FE7}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1232,11 +1234,12 @@
     <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
+    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>104</v>
       </c>
@@ -1277,13 +1280,16 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -1302,14 +1308,14 @@
       <c r="M2" t="s">
         <v>16</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>17</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>106</v>
       </c>
@@ -1328,14 +1334,14 @@
       <c r="M3" t="s">
         <v>22</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>23</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -1354,14 +1360,14 @@
       <c r="M4" t="s">
         <v>27</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>28</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1380,11 +1386,11 @@
       <c r="M5" t="s">
         <v>33</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>108</v>
       </c>
@@ -1403,11 +1409,11 @@
       <c r="M6" t="s">
         <v>22</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -1426,14 +1432,14 @@
       <c r="M7" t="s">
         <v>22</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>23</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -1452,14 +1458,14 @@
       <c r="M8" t="s">
         <v>16</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>17</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>111</v>
       </c>
@@ -1478,11 +1484,11 @@
       <c r="M9" t="s">
         <v>46</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -1501,11 +1507,11 @@
       <c r="M10" t="s">
         <v>22</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -1524,11 +1530,11 @@
       <c r="M11" t="s">
         <v>52</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -1547,11 +1553,11 @@
       <c r="M12" t="s">
         <v>55</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>115</v>
       </c>
@@ -1570,14 +1576,14 @@
       <c r="M13" t="s">
         <v>27</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>58</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>116</v>
       </c>
@@ -1596,14 +1602,14 @@
       <c r="M14" t="s">
         <v>62</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>17</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>117</v>
       </c>
@@ -1622,14 +1628,14 @@
       <c r="M15" t="s">
         <v>22</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>23</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>118</v>
       </c>
@@ -1648,11 +1654,11 @@
       <c r="M16" t="s">
         <v>55</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>119</v>
       </c>
@@ -1671,14 +1677,14 @@
       <c r="M17" t="s">
         <v>22</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>23</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>120</v>
       </c>
@@ -1697,11 +1703,11 @@
       <c r="M18" t="s">
         <v>22</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>121</v>
       </c>
@@ -1720,14 +1726,14 @@
       <c r="M19" t="s">
         <v>74</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>17</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>122</v>
       </c>
@@ -1746,11 +1752,11 @@
       <c r="M20" t="s">
         <v>77</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>123</v>
       </c>
@@ -1769,11 +1775,11 @@
       <c r="M21" t="s">
         <v>22</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>124</v>
       </c>
@@ -1792,11 +1798,11 @@
       <c r="M22" t="s">
         <v>22</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>125</v>
       </c>
@@ -1815,11 +1821,11 @@
       <c r="M23" t="s">
         <v>22</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -1838,11 +1844,11 @@
       <c r="M24" t="s">
         <v>22</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>127</v>
       </c>
@@ -1861,14 +1867,14 @@
       <c r="M25" t="s">
         <v>89</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>23</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -1887,14 +1893,14 @@
       <c r="M26" t="s">
         <v>93</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>17</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -1913,11 +1919,11 @@
       <c r="M27" t="s">
         <v>96</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -1936,14 +1942,14 @@
       <c r="M28" t="s">
         <v>52</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>23</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
         <v>131</v>
       </c>
@@ -1962,10 +1968,10 @@
       <c r="M29" t="s">
         <v>101</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>102</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1974,12 +1980,13 @@
     <hyperlink ref="G1" r:id="rId1" location="property-comments" xr:uid="{C5745B79-2350-9040-A33B-B990DB1FB220}"/>
     <hyperlink ref="L1" r:id="rId2" location="property-super" xr:uid="{C93CACE1-16EA-C64C-B3B5-98BAC468E60A}"/>
     <hyperlink ref="M1" r:id="rId3" location="property-object-gui_element-gui_attributes" xr:uid="{A404F957-34EE-1C45-84B6-64764F3311EA}"/>
-    <hyperlink ref="N1" r:id="rId4" location="property-object-gui_element-gui_attributes" xr:uid="{B488EDE5-F9B6-D249-9B67-4BD8C52BD8DF}"/>
-    <hyperlink ref="O1" r:id="rId5" location="property-object-gui_element-gui_attributes" xr:uid="{A3CD059E-237B-BC4D-A227-4194429C8852}"/>
+    <hyperlink ref="O1" r:id="rId4" location="property-object-gui_element-gui_attributes" xr:uid="{B488EDE5-F9B6-D249-9B67-4BD8C52BD8DF}"/>
+    <hyperlink ref="P1" r:id="rId5" location="property-object-gui_element-gui_attributes" xr:uid="{A3CD059E-237B-BC4D-A227-4194429C8852}"/>
     <hyperlink ref="A1" r:id="rId6" location="property-name" xr:uid="{49D9B3A1-289C-AD44-A8C7-AFCC3397B32D}"/>
     <hyperlink ref="B1" r:id="rId7" location="property-labels" xr:uid="{1C4C342B-22AD-2440-901D-5A8E98EBE39C}"/>
+    <hyperlink ref="N1" r:id="rId8" location="property-subject" xr:uid="{556249D5-670B-2E4F-AD37-1A7B1463E00F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add columns in docs/assets
</commit_message>
<xml_diff>
--- a/docs/assets/data_model_templates/rosetta (rosetta)/properties.xlsx
+++ b/docs/assets/data_model_templates/rosetta (rosetta)/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/docs/assets/data_model_templates/rosetta (rosetta)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools/docs/assets/data_model_templates/rosetta (rosetta)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADD7F20-3DF7-0F4F-A598-8DFEF1279E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5643E5E9-FC52-7242-B49C-080F76F55BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22520" yWindow="5660" windowWidth="27640" windowHeight="16940" xr2:uid="{39EADD64-DA63-9448-899F-8078B27ECEBC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{39EADD64-DA63-9448-899F-8078B27ECEBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,12 +368,65 @@
         </r>
       </text>
     </comment>
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{9C2C0F3B-23D9-EA4D-977C-88C6C02DFDBC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">optional
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">If you have set this project to "public" in the json_header.xlsx, then you can still hide certain properties.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Use "private" to make a property invisible for people outside of your project.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="154">
   <si>
     <t>label_de</t>
   </si>
@@ -829,13 +882,19 @@
   </si>
   <si>
     <t>subject</t>
+  </si>
+  <si>
+    <t>default_permissions_overrule</t>
+  </si>
+  <si>
+    <t>private</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -873,6 +932,12 @@
       <color rgb="FF000000"/>
       <name val="+mn-lt"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -918,10 +983,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -959,7 +1028,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1065,7 +1134,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1207,7 +1276,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1215,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C6BB55-8531-3D43-8AA9-4A28D8869FE7}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1237,9 +1306,10 @@
     <col min="14" max="14" width="13.83203125" customWidth="1"/>
     <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="2" t="s">
         <v>104</v>
       </c>
@@ -1288,8 +1358,11 @@
       <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -1315,7 +1388,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>106</v>
       </c>
@@ -1341,7 +1414,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -1367,7 +1440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1390,7 +1463,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>108</v>
       </c>
@@ -1413,7 +1486,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -1439,7 +1512,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -1465,7 +1538,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>111</v>
       </c>
@@ -1488,7 +1561,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -1511,7 +1584,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -1534,7 +1607,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -1557,7 +1630,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>115</v>
       </c>
@@ -1583,7 +1656,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>116</v>
       </c>
@@ -1609,7 +1682,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>117</v>
       </c>
@@ -1635,7 +1708,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>118</v>
       </c>
@@ -1657,8 +1730,11 @@
       <c r="O16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>119</v>
       </c>
@@ -1684,7 +1760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>120</v>
       </c>
@@ -1707,7 +1783,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>121</v>
       </c>
@@ -1733,7 +1809,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>122</v>
       </c>
@@ -1756,7 +1832,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>123</v>
       </c>
@@ -1779,7 +1855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>124</v>
       </c>
@@ -1802,7 +1878,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>125</v>
       </c>
@@ -1825,7 +1901,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -1848,7 +1924,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
         <v>127</v>
       </c>
@@ -1874,7 +1950,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -1900,7 +1976,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -1923,7 +1999,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -1949,7 +2025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
         <v>131</v>
       </c>
@@ -1973,6 +2049,9 @@
       </c>
       <c r="P29" t="s">
         <v>103</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1985,8 +2064,9 @@
     <hyperlink ref="A1" r:id="rId6" location="property-name" xr:uid="{49D9B3A1-289C-AD44-A8C7-AFCC3397B32D}"/>
     <hyperlink ref="B1" r:id="rId7" location="property-labels" xr:uid="{1C4C342B-22AD-2440-901D-5A8E98EBE39C}"/>
     <hyperlink ref="N1" r:id="rId8" location="property-subject" xr:uid="{556249D5-670B-2E4F-AD37-1A7B1463E00F}"/>
+    <hyperlink ref="Q1" r:id="rId9" location="default_permissions_overrule" xr:uid="{FA1ED5B5-36BB-874F-8176-7C89CA941D7E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(excel2json): add support for overruling default permissions for classes/properties (DEV-5032) (#1915)
</commit_message>
<xml_diff>
--- a/docs/assets/data_model_templates/rosetta (rosetta)/properties.xlsx
+++ b/docs/assets/data_model_templates/rosetta (rosetta)/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/docs/assets/data_model_templates/rosetta (rosetta)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools/docs/assets/data_model_templates/rosetta (rosetta)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADD7F20-3DF7-0F4F-A598-8DFEF1279E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5643E5E9-FC52-7242-B49C-080F76F55BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22520" yWindow="5660" windowWidth="27640" windowHeight="16940" xr2:uid="{39EADD64-DA63-9448-899F-8078B27ECEBC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{39EADD64-DA63-9448-899F-8078B27ECEBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,12 +368,65 @@
         </r>
       </text>
     </comment>
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{9C2C0F3B-23D9-EA4D-977C-88C6C02DFDBC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">optional
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">If you have set this project to "public" in the json_header.xlsx, then you can still hide certain properties.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Use "private" to make a property invisible for people outside of your project.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="154">
   <si>
     <t>label_de</t>
   </si>
@@ -829,13 +882,19 @@
   </si>
   <si>
     <t>subject</t>
+  </si>
+  <si>
+    <t>default_permissions_overrule</t>
+  </si>
+  <si>
+    <t>private</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -873,6 +932,12 @@
       <color rgb="FF000000"/>
       <name val="+mn-lt"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -918,10 +983,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -959,7 +1028,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1065,7 +1134,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1207,7 +1276,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1215,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C6BB55-8531-3D43-8AA9-4A28D8869FE7}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1237,9 +1306,10 @@
     <col min="14" max="14" width="13.83203125" customWidth="1"/>
     <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="2" t="s">
         <v>104</v>
       </c>
@@ -1288,8 +1358,11 @@
       <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -1315,7 +1388,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>106</v>
       </c>
@@ -1341,7 +1414,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -1367,7 +1440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1390,7 +1463,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>108</v>
       </c>
@@ -1413,7 +1486,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -1439,7 +1512,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -1465,7 +1538,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>111</v>
       </c>
@@ -1488,7 +1561,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -1511,7 +1584,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -1534,7 +1607,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -1557,7 +1630,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>115</v>
       </c>
@@ -1583,7 +1656,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>116</v>
       </c>
@@ -1609,7 +1682,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>117</v>
       </c>
@@ -1635,7 +1708,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>118</v>
       </c>
@@ -1657,8 +1730,11 @@
       <c r="O16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>119</v>
       </c>
@@ -1684,7 +1760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>120</v>
       </c>
@@ -1707,7 +1783,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>121</v>
       </c>
@@ -1733,7 +1809,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>122</v>
       </c>
@@ -1756,7 +1832,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>123</v>
       </c>
@@ -1779,7 +1855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>124</v>
       </c>
@@ -1802,7 +1878,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>125</v>
       </c>
@@ -1825,7 +1901,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -1848,7 +1924,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
         <v>127</v>
       </c>
@@ -1874,7 +1950,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -1900,7 +1976,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -1923,7 +1999,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -1949,7 +2025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
         <v>131</v>
       </c>
@@ -1973,6 +2049,9 @@
       </c>
       <c r="P29" t="s">
         <v>103</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1985,8 +2064,9 @@
     <hyperlink ref="A1" r:id="rId6" location="property-name" xr:uid="{49D9B3A1-289C-AD44-A8C7-AFCC3397B32D}"/>
     <hyperlink ref="B1" r:id="rId7" location="property-labels" xr:uid="{1C4C342B-22AD-2440-901D-5A8E98EBE39C}"/>
     <hyperlink ref="N1" r:id="rId8" location="property-subject" xr:uid="{556249D5-670B-2E4F-AD37-1A7B1463E00F}"/>
+    <hyperlink ref="Q1" r:id="rId9" location="default_permissions_overrule" xr:uid="{FA1ED5B5-36BB-874F-8176-7C89CA941D7E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(excel2json)!: remove gui-attributes that do not have an effect in the APP (DEV-5482) (#1985)
</commit_message>
<xml_diff>
--- a/docs/assets/data_model_templates/rosetta (rosetta)/properties.xlsx
+++ b/docs/assets/data_model_templates/rosetta (rosetta)/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools/docs/assets/data_model_templates/rosetta (rosetta)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/docs/assets/data_model_templates/rosetta (rosetta)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5643E5E9-FC52-7242-B49C-080F76F55BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F1F13B-264F-5F4F-9E54-4EDA94A1C417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{39EADD64-DA63-9448-899F-8078B27ECEBC}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="20540" xr2:uid="{39EADD64-DA63-9448-899F-8078B27ECEBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="147">
   <si>
     <t>label_de</t>
   </si>
@@ -482,9 +482,6 @@
     <t>Searchbox</t>
   </si>
   <si>
-    <t>numprops: 1</t>
-  </si>
-  <si>
     <t>Literatur</t>
   </si>
   <si>
@@ -500,9 +497,6 @@
     <t>SimpleText</t>
   </si>
   <si>
-    <t xml:space="preserve">maxlength: 128, size: 128 </t>
-  </si>
-  <si>
     <t>Kategorie</t>
   </si>
   <si>
@@ -548,9 +542,6 @@
     <t>Droits d’auteur</t>
   </si>
   <si>
-    <t xml:space="preserve">maxlength: 128, size: 64 </t>
-  </si>
-  <si>
     <t>Künstler:in</t>
   </si>
   <si>
@@ -602,9 +593,6 @@
     <t>Flatlist</t>
   </si>
   <si>
-    <t>Radio</t>
-  </si>
-  <si>
     <t>hlist: flatlist</t>
   </si>
   <si>
@@ -623,9 +611,6 @@
     <t>Numéro d’inventaire</t>
   </si>
   <si>
-    <t>maxlength: 80, size: 25</t>
-  </si>
-  <si>
     <t>Ort</t>
   </si>
   <si>
@@ -698,9 +683,6 @@
     <t>DecimalValue</t>
   </si>
   <si>
-    <t xml:space="preserve">maxlength: 255, size: 80 </t>
-  </si>
-  <si>
     <t>Aufbewahrende Institution</t>
   </si>
   <si>
@@ -735,9 +717,6 @@
   </si>
   <si>
     <t>Spinbox</t>
-  </si>
-  <si>
-    <t>max: 25.0, min: 0</t>
   </si>
   <si>
     <t>name</t>
@@ -988,9 +967,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1028,7 +1007,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1134,7 +1113,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1276,7 +1255,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1286,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C6BB55-8531-3D43-8AA9-4A28D8869FE7}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1311,10 +1290,10 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1350,7 +1329,7 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>11</v>
@@ -1359,15 +1338,15 @@
         <v>12</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1384,149 +1363,140 @@
       <c r="O2" t="s">
         <v>17</v>
       </c>
-      <c r="P2" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
       <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
         <v>21</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>22</v>
-      </c>
-      <c r="O3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
+      <c r="O4" t="s">
         <v>26</v>
       </c>
-      <c r="L4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="P4" t="s">
         <v>27</v>
-      </c>
-      <c r="O4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" t="s">
         <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" t="s">
         <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L6" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" t="s">
-        <v>22</v>
-      </c>
-      <c r="O6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" t="s">
         <v>21</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>22</v>
-      </c>
-      <c r="O7" t="s">
-        <v>23</v>
-      </c>
-      <c r="P7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M8" t="s">
         <v>16</v>
@@ -1534,524 +1504,497 @@
       <c r="O8" t="s">
         <v>17</v>
       </c>
-      <c r="P8" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" t="s">
+        <v>43</v>
+      </c>
+      <c r="O9" t="s">
         <v>44</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" t="s">
-        <v>46</v>
-      </c>
-      <c r="O9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L10" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" t="s">
         <v>21</v>
       </c>
-      <c r="M10" t="s">
-        <v>22</v>
-      </c>
       <c r="O10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="O11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" t="s">
+        <v>52</v>
+      </c>
+      <c r="O12" t="s">
         <v>53</v>
-      </c>
-      <c r="D12" t="s">
-        <v>54</v>
-      </c>
-      <c r="L12" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" t="s">
-        <v>55</v>
-      </c>
-      <c r="O12" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O13" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="P13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="L14" t="s">
         <v>15</v>
       </c>
       <c r="M14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="O14" t="s">
         <v>17</v>
       </c>
-      <c r="P14" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L15" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" t="s">
         <v>21</v>
       </c>
-      <c r="M15" t="s">
+      <c r="O15" t="s">
         <v>22</v>
-      </c>
-      <c r="O15" t="s">
-        <v>23</v>
-      </c>
-      <c r="P15" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="O16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q16" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="L17" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" t="s">
         <v>21</v>
       </c>
-      <c r="M17" t="s">
+      <c r="O17" t="s">
         <v>22</v>
-      </c>
-      <c r="O17" t="s">
-        <v>23</v>
-      </c>
-      <c r="P17" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="L18" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" t="s">
         <v>21</v>
       </c>
-      <c r="M18" t="s">
-        <v>22</v>
-      </c>
       <c r="O18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="L19" t="s">
         <v>15</v>
       </c>
       <c r="M19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="O19" t="s">
         <v>17</v>
       </c>
-      <c r="P19" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="L20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="O20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="L21" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" t="s">
         <v>21</v>
       </c>
-      <c r="M21" t="s">
-        <v>22</v>
-      </c>
       <c r="O21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L22" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22" t="s">
         <v>21</v>
       </c>
-      <c r="M22" t="s">
-        <v>22</v>
-      </c>
       <c r="O22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B23" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="L23" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" t="s">
         <v>21</v>
       </c>
-      <c r="M23" t="s">
-        <v>22</v>
-      </c>
       <c r="O23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D24" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="L24" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24" t="s">
         <v>21</v>
       </c>
-      <c r="M24" t="s">
-        <v>22</v>
-      </c>
       <c r="O24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="L25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M25" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="O25" t="s">
-        <v>23</v>
-      </c>
-      <c r="P25" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="L26" t="s">
         <v>15</v>
       </c>
       <c r="M26" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="O26" t="s">
         <v>17</v>
       </c>
-      <c r="P26" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="L27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M27" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="O27" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D28" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="L28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M28" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="O28" t="s">
-        <v>23</v>
-      </c>
-      <c r="P28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B29" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D29" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M29" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="O29" t="s">
-        <v>102</v>
-      </c>
-      <c r="P29" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="Q29" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>